<commit_message>
v0.5.1 - page numbering
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
+++ b/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.0</t>
+    <t>0.5.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-25T11:43:35-07:00</t>
+    <t>2025-12-29T13:16:13-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
v0.5.2 - page references
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
+++ b/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.1</t>
+    <t>0.5.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-29T13:16:13-07:00</t>
+    <t>2025-12-29T20:17:52-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
v0.5.3 - ValueSets and CodeSystems
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
+++ b/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.2</t>
+    <t>0.5.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-29T20:17:52-07:00</t>
+    <t>2025-12-29T22:23:37-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
v0.5.4 - artemis missions; scientific symbols
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
+++ b/docs/CodeSystem-aerospace-behavioral-state-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.3</t>
+    <t>0.5.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-29T22:23:37-07:00</t>
+    <t>2025-12-29T23:18:22-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>